<commit_message>
Fed data for retail vs wholesale proxy
</commit_message>
<xml_diff>
--- a/raw_data/Fed_CO_2000Q1_2025Q4.xlsx
+++ b/raw_data/Fed_CO_2000Q1_2025Q4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohamjoshi/Desktop/Spring Project/Raw Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohamjoshi/Desktop/Spring Project/Codes/fim601-ccar/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53465879-2719-AC4C-A32B-C637319725D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E02699-364F-4742-A0BB-B632EE218C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1580" windowWidth="28040" windowHeight="17180" xr2:uid="{0DAE4272-EAFD-B04A-B681-E0124C690E7A}"/>
+    <workbookView xWindow="4220" yWindow="1580" windowWidth="28040" windowHeight="17180" xr2:uid="{0DAE4272-EAFD-B04A-B681-E0124C690E7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1485,12 +1485,13 @@
   <dimension ref="A1:W110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="6"/>
     <col min="9" max="9" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
@@ -1501,6 +1502,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
@@ -1513,7 +1515,7 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
@@ -1584,7 +1586,7 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E3" t="s">
@@ -1655,7 +1657,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
       <c r="E4">
@@ -1726,7 +1728,7 @@
       <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
@@ -1797,7 +1799,7 @@
       <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E6" t="s">
@@ -1868,7 +1870,7 @@
       <c r="C7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1939,7 +1941,7 @@
       <c r="C8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>0.59</v>
       </c>
       <c r="E8">
@@ -2010,7 +2012,7 @@
       <c r="C9">
         <v>0.25</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>0.7</v>
       </c>
       <c r="E9">
@@ -2081,7 +2083,7 @@
       <c r="C10">
         <v>0.63</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>0.71</v>
       </c>
       <c r="E10">
@@ -2152,7 +2154,7 @@
       <c r="C11">
         <v>0.84</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>0.98</v>
       </c>
       <c r="E11">
@@ -2223,7 +2225,7 @@
       <c r="C12">
         <v>1.4</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>1.1100000000000001</v>
       </c>
       <c r="E12">
@@ -2294,7 +2296,7 @@
       <c r="C13">
         <v>0.87</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="6">
         <v>1.28</v>
       </c>
       <c r="E13">
@@ -2365,7 +2367,7 @@
       <c r="C14">
         <v>1.71</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>1.54</v>
       </c>
       <c r="E14">
@@ -2436,7 +2438,7 @@
       <c r="C15">
         <v>0.33</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>1.85</v>
       </c>
       <c r="E15">
@@ -2507,7 +2509,7 @@
       <c r="C16">
         <v>0.75</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>1.82</v>
       </c>
       <c r="E16">
@@ -2578,7 +2580,7 @@
       <c r="C17">
         <v>0.86</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>2.0699999999999998</v>
       </c>
       <c r="E17">
@@ -2649,7 +2651,7 @@
       <c r="C18">
         <v>0.82</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>2.5099999999999998</v>
       </c>
       <c r="E18">
@@ -2720,7 +2722,7 @@
       <c r="C19">
         <v>1.04</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>1.45</v>
       </c>
       <c r="E19">
@@ -2791,7 +2793,7 @@
       <c r="C20">
         <v>0.47</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="6">
         <v>1.84</v>
       </c>
       <c r="E20">
@@ -2862,7 +2864,7 @@
       <c r="C21">
         <v>0.19</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>1.56</v>
       </c>
       <c r="E21">
@@ -2933,7 +2935,7 @@
       <c r="C22">
         <v>0.46</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="6">
         <v>1.38</v>
       </c>
       <c r="E22">
@@ -3004,7 +3006,7 @@
       <c r="C23">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="6">
         <v>0.87</v>
       </c>
       <c r="E23">
@@ -3075,7 +3077,7 @@
       <c r="C24">
         <v>0.44</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="6">
         <v>0.84</v>
       </c>
       <c r="E24">
@@ -3146,7 +3148,7 @@
       <c r="C25">
         <v>0.46</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="6">
         <v>0.57999999999999996</v>
       </c>
       <c r="E25">
@@ -3217,7 +3219,7 @@
       <c r="C26">
         <v>0.22</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="6">
         <v>0.38</v>
       </c>
       <c r="E26">
@@ -3288,7 +3290,7 @@
       <c r="C27">
         <v>-0.16</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="6">
         <v>0.31</v>
       </c>
       <c r="E27">
@@ -3359,7 +3361,7 @@
       <c r="C28">
         <v>0.08</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="6">
         <v>0.2</v>
       </c>
       <c r="E28">
@@ -3430,7 +3432,7 @@
       <c r="C29">
         <v>0.12</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="6">
         <v>0.17</v>
       </c>
       <c r="E29">
@@ -3501,7 +3503,7 @@
       <c r="C30">
         <v>0.03</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="6">
         <v>0.12</v>
       </c>
       <c r="E30">
@@ -3572,7 +3574,7 @@
       <c r="C31">
         <v>-0.18</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="6">
         <v>0.26</v>
       </c>
       <c r="E31">
@@ -3643,7 +3645,7 @@
       <c r="C32">
         <v>0.22</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="6">
         <v>0.17</v>
       </c>
       <c r="E32">
@@ -3714,7 +3716,7 @@
       <c r="C33">
         <v>0.15</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="6">
         <v>0.21</v>
       </c>
       <c r="E33">
@@ -3785,7 +3787,7 @@
       <c r="C34">
         <v>0.02</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="6">
         <v>0.26</v>
       </c>
       <c r="E34">
@@ -3856,7 +3858,7 @@
       <c r="C35">
         <v>0.2</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="6">
         <v>0.28999999999999998</v>
       </c>
       <c r="E35">
@@ -3927,7 +3929,7 @@
       <c r="C36">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="6">
         <v>0.35</v>
       </c>
       <c r="E36">
@@ -3998,7 +4000,7 @@
       <c r="C37">
         <v>0.12</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="6">
         <v>0.41</v>
       </c>
       <c r="E37">
@@ -4069,7 +4071,7 @@
       <c r="C38">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="6">
         <v>0.43</v>
       </c>
       <c r="E38">
@@ -4140,7 +4142,7 @@
       <c r="C39">
         <v>0.02</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="6">
         <v>0.67</v>
       </c>
       <c r="E39">
@@ -4211,7 +4213,7 @@
       <c r="C40">
         <v>0.09</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="6">
         <v>0.72</v>
       </c>
       <c r="E40">
@@ -4282,7 +4284,7 @@
       <c r="C41">
         <v>0.27</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="6">
         <v>0.84</v>
       </c>
       <c r="E41">
@@ -4353,7 +4355,7 @@
       <c r="C42">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="6">
         <v>1.02</v>
       </c>
       <c r="E42">
@@ -4424,7 +4426,7 @@
       <c r="C43">
         <v>0.26</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="6">
         <v>1.29</v>
       </c>
       <c r="E43">
@@ -4495,7 +4497,7 @@
       <c r="C44">
         <v>0.51</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="6">
         <v>2</v>
       </c>
       <c r="E44">
@@ -4566,7 +4568,7 @@
       <c r="C45">
         <v>0.65</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="6">
         <v>2.4700000000000002</v>
       </c>
       <c r="E45">
@@ -4637,7 +4639,7 @@
       <c r="C46">
         <v>0.99</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="6">
         <v>2.67</v>
       </c>
       <c r="E46">
@@ -4708,7 +4710,7 @@
       <c r="C47">
         <v>1.02</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="6">
         <v>2.3199999999999998</v>
       </c>
       <c r="E47">
@@ -4779,7 +4781,7 @@
       <c r="C48">
         <v>2.88</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="6">
         <v>2.11</v>
       </c>
       <c r="E48">
@@ -4850,7 +4852,7 @@
       <c r="C49">
         <v>1.17</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="6">
         <v>1.9</v>
       </c>
       <c r="E49">
@@ -4921,7 +4923,7 @@
       <c r="C50">
         <v>1.98</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="6">
         <v>1.71</v>
       </c>
       <c r="E50">
@@ -4992,7 +4994,7 @@
       <c r="C51">
         <v>1.99</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="6">
         <v>1.26</v>
       </c>
       <c r="E51">
@@ -5063,7 +5065,7 @@
       <c r="C52">
         <v>1.1100000000000001</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="6">
         <v>1.1399999999999999</v>
       </c>
       <c r="E52">
@@ -5134,7 +5136,7 @@
       <c r="C53">
         <v>0.54</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="6">
         <v>0.78</v>
       </c>
       <c r="E53">
@@ -5205,7 +5207,7 @@
       <c r="C54">
         <v>0.3</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="6">
         <v>0.66</v>
       </c>
       <c r="E54">
@@ -5276,7 +5278,7 @@
       <c r="C55">
         <v>0.17</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="6">
         <v>0.62</v>
       </c>
       <c r="E55">
@@ -5347,7 +5349,7 @@
       <c r="C56">
         <v>0.45</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="6">
         <v>0.51</v>
       </c>
       <c r="E56">
@@ -5418,7 +5420,7 @@
       <c r="C57">
         <v>0.78</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="6">
         <v>0.49</v>
       </c>
       <c r="E57">
@@ -5489,7 +5491,7 @@
       <c r="C58">
         <v>0.6</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="6">
         <v>0.43</v>
       </c>
       <c r="E58">
@@ -5560,7 +5562,7 @@
       <c r="C59">
         <v>0.7</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="6">
         <v>0.27</v>
       </c>
       <c r="E59">
@@ -5631,7 +5633,7 @@
       <c r="C60">
         <v>-0.1</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="6">
         <v>0.33</v>
       </c>
       <c r="E60">
@@ -5702,7 +5704,7 @@
       <c r="C61">
         <v>0.01</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="6">
         <v>0.27</v>
       </c>
       <c r="E61">
@@ -5773,7 +5775,7 @@
       <c r="C62">
         <v>0.32</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="6">
         <v>0.24</v>
       </c>
       <c r="E62">
@@ -5844,7 +5846,7 @@
       <c r="C63">
         <v>0.05</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="6">
         <v>0.22</v>
       </c>
       <c r="E63">
@@ -5915,7 +5917,7 @@
       <c r="C64">
         <v>0.12</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="6">
         <v>0.21</v>
       </c>
       <c r="E64">
@@ -5986,7 +5988,7 @@
       <c r="C65">
         <v>0.04</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="6">
         <v>0.18</v>
       </c>
       <c r="E65">
@@ -6057,7 +6059,7 @@
       <c r="C66">
         <v>-0.05</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="6">
         <v>0.18</v>
       </c>
       <c r="E66">
@@ -6128,7 +6130,7 @@
       <c r="C67">
         <v>-0.03</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="6">
         <v>0.21</v>
       </c>
       <c r="E67">
@@ -6199,7 +6201,7 @@
       <c r="C68">
         <v>0.03</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="6">
         <v>0.16</v>
       </c>
       <c r="E68">
@@ -6270,7 +6272,7 @@
       <c r="C69">
         <v>0.15</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="6">
         <v>0.21</v>
       </c>
       <c r="E69">
@@ -6341,7 +6343,7 @@
       <c r="C70">
         <v>0.02</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="6">
         <v>0.24</v>
       </c>
       <c r="E70">
@@ -6412,7 +6414,7 @@
       <c r="C71">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="6">
         <v>0.31</v>
       </c>
       <c r="E71">
@@ -6483,7 +6485,7 @@
       <c r="C72">
         <v>0.39</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="6">
         <v>0.43</v>
       </c>
       <c r="E72">
@@ -6554,7 +6556,7 @@
       <c r="C73">
         <v>0.24</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="6">
         <v>0.44</v>
       </c>
       <c r="E73">
@@ -6625,7 +6627,7 @@
       <c r="C74">
         <v>0.15</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="6">
         <v>0.44</v>
       </c>
       <c r="E74">
@@ -6696,7 +6698,7 @@
       <c r="C75">
         <v>0.37</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="6">
         <v>0.38</v>
       </c>
       <c r="E75">
@@ -6767,7 +6769,7 @@
       <c r="C76">
         <v>0.27</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="6">
         <v>0.32</v>
       </c>
       <c r="E76">
@@ -6838,7 +6840,7 @@
       <c r="C77">
         <v>0.44</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="6">
         <v>0.36</v>
       </c>
       <c r="E77">
@@ -6909,7 +6911,7 @@
       <c r="C78">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="6">
         <v>0.32</v>
       </c>
       <c r="E78">
@@ -6980,7 +6982,7 @@
       <c r="C79">
         <v>0.35</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="6">
         <v>0.34</v>
       </c>
       <c r="E79">
@@ -7051,7 +7053,7 @@
       <c r="C80">
         <v>0.33</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="6">
         <v>0.28000000000000003</v>
       </c>
       <c r="E80">
@@ -7122,7 +7124,7 @@
       <c r="C81">
         <v>0.48</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="6">
         <v>0.24</v>
       </c>
       <c r="E81">
@@ -7193,7 +7195,7 @@
       <c r="C82">
         <v>0.92</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="6">
         <v>0.24</v>
       </c>
       <c r="E82">
@@ -7264,7 +7266,7 @@
       <c r="C83">
         <v>-0.02</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="6">
         <v>0.27</v>
       </c>
       <c r="E83">
@@ -7335,7 +7337,7 @@
       <c r="C84">
         <v>0.39</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="6">
         <v>0.28999999999999998</v>
       </c>
       <c r="E84">
@@ -7406,7 +7408,7 @@
       <c r="C85">
         <v>0.26</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="6">
         <v>0.3</v>
       </c>
       <c r="E85">
@@ -7477,7 +7479,7 @@
       <c r="C86">
         <v>0.21</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="6">
         <v>0.42</v>
       </c>
       <c r="E86">
@@ -7548,7 +7550,7 @@
       <c r="C87">
         <v>0.35</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="6">
         <v>0.37</v>
       </c>
       <c r="E87">
@@ -7619,7 +7621,7 @@
       <c r="C88">
         <v>0.25</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="6">
         <v>0.56000000000000005</v>
       </c>
       <c r="E88">
@@ -7690,7 +7692,7 @@
       <c r="C89">
         <v>0.36</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="6">
         <v>0.63</v>
       </c>
       <c r="E89">
@@ -7761,7 +7763,7 @@
       <c r="C90">
         <v>0.98</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="6">
         <v>0.55000000000000004</v>
       </c>
       <c r="E90">
@@ -7832,7 +7834,7 @@
       <c r="C91">
         <v>0.41</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="6">
         <v>0.46</v>
       </c>
       <c r="E91">
@@ -7903,7 +7905,7 @@
       <c r="C92">
         <v>0.04</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="6">
         <v>0.3</v>
       </c>
       <c r="E92">
@@ -7974,7 +7976,7 @@
       <c r="C93">
         <v>-0.03</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="6">
         <v>0.22</v>
       </c>
       <c r="E93">
@@ -8045,7 +8047,7 @@
       <c r="C94">
         <v>-0.11</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="6">
         <v>0.16</v>
       </c>
       <c r="E94">
@@ -8116,7 +8118,7 @@
       <c r="C95">
         <v>-0.08</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="6">
         <v>0.1</v>
       </c>
       <c r="E95">
@@ -8187,7 +8189,7 @@
       <c r="C96">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="6">
         <v>0.12</v>
       </c>
       <c r="E96">
@@ -8258,7 +8260,7 @@
       <c r="C97">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="6">
         <v>0.14000000000000001</v>
       </c>
       <c r="E97">
@@ -8329,7 +8331,7 @@
       <c r="C98">
         <v>-0.09</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="6">
         <v>0.16</v>
       </c>
       <c r="E98">
@@ -8400,7 +8402,7 @@
       <c r="C99">
         <v>-0.05</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="6">
         <v>0.24</v>
       </c>
       <c r="E99">
@@ -8471,7 +8473,7 @@
       <c r="C100">
         <v>0.36</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="6">
         <v>0.27</v>
       </c>
       <c r="E100">
@@ -8542,7 +8544,7 @@
       <c r="C101">
         <v>-0.06</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="6">
         <v>0.31</v>
       </c>
       <c r="E101">
@@ -8613,7 +8615,7 @@
       <c r="C102">
         <v>0.06</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="6">
         <v>0.38</v>
       </c>
       <c r="E102">
@@ -8684,7 +8686,7 @@
       <c r="C103">
         <v>0.12</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="6">
         <v>0.42</v>
       </c>
       <c r="E103">
@@ -8755,7 +8757,7 @@
       <c r="C104">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="6">
         <v>0.44</v>
       </c>
       <c r="E104">
@@ -8826,7 +8828,7 @@
       <c r="C105">
         <v>1.05</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="6">
         <v>0.48</v>
       </c>
       <c r="E105">
@@ -8897,7 +8899,7 @@
       <c r="C106">
         <v>0.12</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="6">
         <v>0.56999999999999995</v>
       </c>
       <c r="E106">
@@ -8968,7 +8970,7 @@
       <c r="C107">
         <v>1.05</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="6">
         <v>0.5</v>
       </c>
       <c r="E107">
@@ -9039,7 +9041,7 @@
       <c r="C108">
         <v>0.36</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="6">
         <v>0.56000000000000005</v>
       </c>
       <c r="E108">
@@ -9110,7 +9112,7 @@
       <c r="C109">
         <v>0.31</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="6">
         <v>0.57999999999999996</v>
       </c>
       <c r="E109">
@@ -9181,7 +9183,7 @@
       <c r="C110">
         <v>0.15</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="6">
         <v>0.57999999999999996</v>
       </c>
       <c r="E110">

</xml_diff>